<commit_message>
Update data analysis notebooks and synthetic data
</commit_message>
<xml_diff>
--- a/CHATGPT - STARTERS PACKAGE/New synthetic data/Synthetic_simulated_cases_selected_all.xlsx
+++ b/CHATGPT - STARTERS PACKAGE/New synthetic data/Synthetic_simulated_cases_selected_all.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,7 +665,7 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>15.16307318277267</v>
+        <v>15.1610087863751</v>
       </c>
     </row>
     <row r="9">
@@ -695,7 +695,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>11.74293186326184</v>
+        <v>11.81293910030774</v>
       </c>
     </row>
     <row r="10">
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>10.9298645993533</v>
+        <v>10.85437886210314</v>
       </c>
     </row>
     <row r="11">
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>14.86035783521515</v>
+        <v>14.83900377952033</v>
       </c>
     </row>
     <row r="12">
@@ -763,7 +763,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>2250</v>
+        <v>2500</v>
       </c>
       <c r="C12" t="n">
         <v>34</v>
@@ -773,11 +773,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Config_162</t>
+          <t>Config_198</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>48.66558175</v>
+        <v>45.45433982</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -785,7 +785,7 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>12.78157748750503</v>
+        <v>12.74190179965575</v>
       </c>
     </row>
     <row r="13">
@@ -815,7 +815,7 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>11.43920422575733</v>
+        <v>11.19937228142982</v>
       </c>
     </row>
     <row r="14">
@@ -829,15 +829,15 @@
         <v>22</v>
       </c>
       <c r="D14" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Config_153</t>
+          <t>Config_152</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>33.78345127</v>
+        <v>33.91581593</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>15.80993418709444</v>
+        <v>15.72664406951813</v>
       </c>
     </row>
     <row r="15">
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>12.55734617185913</v>
+        <v>12.64418896608578</v>
       </c>
     </row>
     <row r="16">
@@ -905,67 +905,7 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>10.61477224022275</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C17" t="n">
-        <v>34</v>
-      </c>
-      <c r="D17" t="n">
-        <v>10</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Config_193</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>20.75618301</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>BO</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>9.698617927826017</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="n">
-        <v>2500</v>
-      </c>
-      <c r="C18" t="n">
-        <v>10</v>
-      </c>
-      <c r="D18" t="n">
-        <v>10</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Config_181</t>
-        </is>
-      </c>
-      <c r="F18" t="n">
-        <v>53.98288219</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>BO</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>12.78625908389365</v>
+        <v>10.21370698986457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>